<commit_message>
Array  introduced for parameters
</commit_message>
<xml_diff>
--- a/main/app/brm_core/BRMRulesInRows.xlsx
+++ b/main/app/brm_core/BRMRulesInRows.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t>None</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Length,Weight</t>
   </si>
   <si>
-    <t>Sum_of(CushionDB)&lt;30</t>
-  </si>
-  <si>
     <t>Sum_of(Length) &lt;600</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>##### Hazardouse neighbours occure ######</t>
+  </si>
+  <si>
+    <t>CushionDB=[36,35]</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -560,10 +560,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="3">
         <v>0</v>
@@ -601,18 +601,18 @@
     </row>
     <row r="2" spans="1:17" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
@@ -648,18 +648,16 @@
     </row>
     <row r="3" spans="1:17" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>0</v>
@@ -697,7 +695,7 @@
     </row>
     <row r="4" spans="1:17" ht="30.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -706,7 +704,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>0</v>
@@ -744,18 +742,18 @@
     </row>
     <row r="5" spans="1:17" ht="30.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed a lot of bugs introduce new one :-) . New sintax: ['a','b']
</commit_message>
<xml_diff>
--- a/main/app/brm_core/BRMRulesInRows.xlsx
+++ b/main/app/brm_core/BRMRulesInRows.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,14 +67,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>CushionDB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sum_of(Weight)/Sum_of(Length) &gt; 1 </t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>CushionDB=[36,35]</t>
+  </si>
+  <si>
+    <t>CushionDB,BEARINGS</t>
+  </si>
+  <si>
+    <t>BEARINGS=['A','B']</t>
   </si>
 </sst>
 </file>
@@ -537,82 +540,82 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="4" max="5" width="23.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3">
+        <v>0</v>
+      </c>
+      <c r="I1" s="3">
+        <v>0</v>
+      </c>
+      <c r="J1" s="3">
+        <v>0</v>
+      </c>
+      <c r="K1" s="3">
+        <v>0</v>
+      </c>
+      <c r="L1" s="3">
+        <v>0</v>
+      </c>
+      <c r="M1" s="3">
+        <v>0</v>
+      </c>
+      <c r="N1" s="3">
+        <v>0</v>
+      </c>
+      <c r="O1" s="3">
+        <v>0</v>
+      </c>
+      <c r="P1" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="3">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3">
-        <v>0</v>
-      </c>
-      <c r="I1" s="3">
-        <v>0</v>
-      </c>
-      <c r="J1" s="3">
-        <v>0</v>
-      </c>
-      <c r="K1" s="3">
-        <v>0</v>
-      </c>
-      <c r="L1" s="3">
-        <v>0</v>
-      </c>
-      <c r="M1" s="3">
-        <v>0</v>
-      </c>
-      <c r="N1" s="3">
-        <v>0</v>
-      </c>
-      <c r="O1" s="3">
-        <v>0</v>
-      </c>
-      <c r="P1" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
@@ -646,18 +649,18 @@
       </c>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>0</v>
@@ -693,18 +696,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>0</v>
@@ -740,20 +745,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>0</v>
@@ -789,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>